<commit_message>
edits to work on the latest ig-pub and worke on the prefetch narrative
</commit_message>
<xml_diff>
--- a/docs/argo-appt.xlsx
+++ b/docs/argo-appt.xlsx
@@ -174,7 +174,7 @@
     <t>Y</t>
   </si>
   <si>
-    <t xml:space="preserve">id
+    <t xml:space="preserve">id {[]} {[]}
 </t>
   </si>
   <si>
@@ -193,7 +193,7 @@
     <t>Appointment.meta</t>
   </si>
   <si>
-    <t xml:space="preserve">Meta
+    <t xml:space="preserve">Meta {[]} {[]}
 </t>
   </si>
   <si>
@@ -209,7 +209,7 @@
     <t>Appointment.implicitRules</t>
   </si>
   <si>
-    <t xml:space="preserve">uri
+    <t xml:space="preserve">uri {[]} {[]}
 </t>
   </si>
   <si>
@@ -229,7 +229,7 @@
     <t>Appointment.language</t>
   </si>
   <si>
-    <t xml:space="preserve">code
+    <t xml:space="preserve">code {[]} {[]}
 </t>
   </si>
   <si>
@@ -261,7 +261,7 @@
 htmlxhtmldisplay</t>
   </si>
   <si>
-    <t xml:space="preserve">Narrative
+    <t xml:space="preserve">Narrative {[]} {[]}
 </t>
   </si>
   <si>
@@ -291,7 +291,7 @@
 anonymous resourcescontained resources</t>
   </si>
   <si>
-    <t xml:space="preserve">Resource
+    <t xml:space="preserve">Resource {[]} {[]}
 </t>
   </si>
   <si>
@@ -313,7 +313,7 @@
     <t>Appointment.extension</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension
+    <t xml:space="preserve">Extension {[]} {[]}
 </t>
   </si>
   <si>
@@ -336,7 +336,7 @@
     <t>status-reason-extension</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://fhir.org/guides/argonaut-scheduling/StructureDefinition/extension-status-reason}
+    <t xml:space="preserve">Extension {[CanonicalType[http://fhir.org/guides/argonaut-scheduling/StructureDefinition/extension-status-reason]]} {[]}
 </t>
   </si>
   <si>
@@ -370,7 +370,7 @@
     <t>Appointment.identifier</t>
   </si>
   <si>
-    <t xml:space="preserve">Identifier
+    <t xml:space="preserve">Identifier {[]} {[]}
 </t>
   </si>
   <si>
@@ -426,7 +426,7 @@
     <t>Appointment.serviceCategory</t>
   </si>
   <si>
-    <t xml:space="preserve">CodeableConcept
+    <t xml:space="preserve">CodeableConcept {[]} {[]}
 </t>
   </si>
   <si>
@@ -524,8 +524,8 @@
     <t>Appointment.indication</t>
   </si>
   <si>
-    <t>Reference {http://hl7.org/fhir/StructureDefinition/Condition}
-Reference {http://hl7.org/fhir/StructureDefinition/Procedure}</t>
+    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Condition], CanonicalType[http://hl7.org/fhir/StructureDefinition/Procedure]]}
+</t>
   </si>
   <si>
     <t>Reason the appointment is to takes place (resource)</t>
@@ -540,7 +540,7 @@
     <t>Appointment.priority</t>
   </si>
   <si>
-    <t xml:space="preserve">unsignedInt
+    <t xml:space="preserve">unsignedInt {[]} {[]}
 </t>
   </si>
   <si>
@@ -567,7 +567,7 @@
     <t>Appointment.description</t>
   </si>
   <si>
-    <t xml:space="preserve">string
+    <t xml:space="preserve">string {[]} {[]}
 </t>
   </si>
   <si>
@@ -589,7 +589,7 @@
     <t>Appointment.supportingInformation</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {http://hl7.org/fhir/StructureDefinition/Resource}
+    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Resource]]}
 </t>
   </si>
   <si>
@@ -608,7 +608,7 @@
     <t>Appointment.start</t>
   </si>
   <si>
-    <t xml:space="preserve">instant
+    <t xml:space="preserve">instant {[]} {[]}
 </t>
   </si>
   <si>
@@ -648,7 +648,7 @@
     <t>Appointment.minutesDuration</t>
   </si>
   <si>
-    <t xml:space="preserve">positiveInt
+    <t xml:space="preserve">positiveInt {[]} {[]}
 </t>
   </si>
   <si>
@@ -664,7 +664,7 @@
     <t>Appointment.slot</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {http://hl7.org/fhir/StructureDefinition/Slot}
+    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Slot]]}
 </t>
   </si>
   <si>
@@ -680,7 +680,7 @@
     <t>Appointment.created</t>
   </si>
   <si>
-    <t xml:space="preserve">dateTime
+    <t xml:space="preserve">dateTime {[]} {[]}
 </t>
   </si>
   <si>
@@ -719,7 +719,7 @@
     <t>Appointment.incomingReferral</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {http://hl7.org/fhir/StructureDefinition/ReferralRequest}
+    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/ReferralRequest]]}
 </t>
   </si>
   <si>
@@ -738,7 +738,7 @@
     <t>p-1</t>
   </si>
   <si>
-    <t xml:space="preserve">BackboneElement
+    <t xml:space="preserve">BackboneElement {[]} {[]}
 </t>
   </si>
   <si>
@@ -832,8 +832,8 @@
     <t>Appointment.participant.actor</t>
   </si>
   <si>
-    <t>Reference {http://hl7.org/fhir/us/core/StructureDefinition/us-core-location}
-Reference {http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient}Reference {http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitioner}Reference {http://hl7.org/fhir/StructureDefinition/HealthcareService}</t>
+    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/us/core/StructureDefinition/us-core-location], CanonicalType[http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient], CanonicalType[http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitioner], CanonicalType[http://hl7.org/fhir/StructureDefinition/HealthcareService]]}
+</t>
   </si>
   <si>
     <t>Person, Location/HealthcareService or Device</t>
@@ -902,7 +902,7 @@
     <t>Appointment.requestedPeriod</t>
   </si>
   <si>
-    <t xml:space="preserve">Period
+    <t xml:space="preserve">Period {[]} {[]}
 </t>
   </si>
   <si>

</xml_diff>